<commit_message>
Improved schematics and routing of 5V-5V board. Generated PDF schematics. Generated PNG preview. Generated CAM files.
</commit_message>
<xml_diff>
--- a/doc/TPS63020 Calculator.xlsx
+++ b/doc/TPS63020 Calculator.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AG\Documents\EAGLE\projects\DC-DC\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7370355D-6F58-4F5B-A563-FCBCEBC5EA5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1467B249-0CD1-4060-8C8F-4748CA05F5D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1140" yWindow="1050" windowWidth="17320" windowHeight="19950" xr2:uid="{D6F40B62-0C07-4D06-9576-817CE55B7C65}"/>
   </bookViews>
@@ -423,7 +423,7 @@
   <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -639,7 +639,7 @@
         <v>5</v>
       </c>
       <c r="H9" s="2">
-        <v>1600000</v>
+        <v>1620000</v>
       </c>
       <c r="I9" t="s">
         <v>1</v>
@@ -649,7 +649,7 @@
       </c>
       <c r="K9">
         <f>($H9/$B$4+1)*$B$3</f>
-        <v>4.9444444444444446</v>
+        <v>5</v>
       </c>
       <c r="L9" t="s">
         <v>0</v>

</xml_diff>

<commit_message>
Added 200k resistor to improve voltage output. Generated CAM files. Generated PNG preview. Generated PDF schematics. Adjusted BoM and PnP files. Adjusted Excel calculator.
</commit_message>
<xml_diff>
--- a/doc/TPS63020 Calculator.xlsx
+++ b/doc/TPS63020 Calculator.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AG\Documents\EAGLE\projects\DC-DC\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1467B249-0CD1-4060-8C8F-4748CA05F5D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEBDE16E-34A9-4415-9013-E50916BA31FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1140" yWindow="1050" windowWidth="17320" windowHeight="19950" xr2:uid="{D6F40B62-0C07-4D06-9576-817CE55B7C65}"/>
+    <workbookView xWindow="790" yWindow="960" windowWidth="17320" windowHeight="19950" xr2:uid="{D6F40B62-0C07-4D06-9576-817CE55B7C65}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -423,7 +423,7 @@
   <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -519,7 +519,8 @@
         <v>5</v>
       </c>
       <c r="H6" s="2">
-        <v>1000000</v>
+        <f>1000000+20000</f>
+        <v>1020000</v>
       </c>
       <c r="I6" t="s">
         <v>1</v>
@@ -529,7 +530,7 @@
       </c>
       <c r="K6">
         <f>($H6/$B$4+1)*$B$3</f>
-        <v>3.2777777777777777</v>
+        <v>3.3333333333333335</v>
       </c>
       <c r="L6" t="s">
         <v>0</v>
@@ -639,7 +640,8 @@
         <v>5</v>
       </c>
       <c r="H9" s="2">
-        <v>1620000</v>
+        <f>1000000+20000+620000</f>
+        <v>1640000</v>
       </c>
       <c r="I9" t="s">
         <v>1</v>
@@ -649,7 +651,7 @@
       </c>
       <c r="K9">
         <f>($H9/$B$4+1)*$B$3</f>
-        <v>5</v>
+        <v>5.0555555555555554</v>
       </c>
       <c r="L9" t="s">
         <v>0</v>

</xml_diff>

<commit_message>
Added new step-up/down board. Generated CAM files. Generated PNG preview. Generated PDF schematics. Generated BoM and PnP files. Updated descriptions. Updated XLS calculator.
</commit_message>
<xml_diff>
--- a/doc/TPS63020 Calculator.xlsx
+++ b/doc/TPS63020 Calculator.xlsx
@@ -1,31 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AG\Documents\EAGLE\projects\DC-DC\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEBDE16E-34A9-4415-9013-E50916BA31FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BB16DA6-3064-41AA-9C7F-9100A0F1217B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="790" yWindow="960" windowWidth="17320" windowHeight="19950" xr2:uid="{D6F40B62-0C07-4D06-9576-817CE55B7C65}"/>
+    <workbookView xWindow="60" yWindow="100" windowWidth="18080" windowHeight="20730" xr2:uid="{D6F40B62-0C07-4D06-9576-817CE55B7C65}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="12">
   <si>
     <t>V</t>
   </si>
@@ -52,6 +59,15 @@
   </si>
   <si>
     <t>Vfb (fix)</t>
+  </si>
+  <si>
+    <t>C22984</t>
+  </si>
+  <si>
+    <t>C128551</t>
+  </si>
+  <si>
+    <t>C31850</t>
   </si>
 </sst>
 </file>
@@ -420,20 +436,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98303E75-3625-4237-82B0-3A63F73F1B04}">
-  <dimension ref="A1:L9"/>
+  <dimension ref="A1:N14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:12" ht="26" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:14" ht="26" x14ac:dyDescent="0.6">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -444,7 +458,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -455,7 +469,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -495,7 +509,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -536,7 +550,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -576,7 +590,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -616,7 +630,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -655,6 +669,110 @@
       </c>
       <c r="L9" t="s">
         <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="2">
+        <v>22000</v>
+      </c>
+      <c r="C12" t="s">
+        <v>1</v>
+      </c>
+      <c r="M12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" s="2">
+        <v>1.2</v>
+      </c>
+      <c r="C13" t="s">
+        <v>0</v>
+      </c>
+      <c r="D13" t="s">
+        <v>4</v>
+      </c>
+      <c r="E13">
+        <f>$B$12*($B13/$B$3-1)</f>
+        <v>30799.999999999996</v>
+      </c>
+      <c r="F13" t="s">
+        <v>1</v>
+      </c>
+      <c r="G13" t="s">
+        <v>5</v>
+      </c>
+      <c r="H13" s="2">
+        <v>30000</v>
+      </c>
+      <c r="I13" t="s">
+        <v>1</v>
+      </c>
+      <c r="J13" t="s">
+        <v>2</v>
+      </c>
+      <c r="K13">
+        <f>($H13/$B$12+1)*$B$3</f>
+        <v>1.1818181818181817</v>
+      </c>
+      <c r="L13" t="s">
+        <v>0</v>
+      </c>
+      <c r="M13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" s="2">
+        <v>5.5</v>
+      </c>
+      <c r="C14" t="s">
+        <v>0</v>
+      </c>
+      <c r="D14" t="s">
+        <v>4</v>
+      </c>
+      <c r="E14">
+        <f>$B$12*($B14/$B$3-1)</f>
+        <v>220000</v>
+      </c>
+      <c r="F14" t="s">
+        <v>1</v>
+      </c>
+      <c r="G14" t="s">
+        <v>5</v>
+      </c>
+      <c r="H14" s="2">
+        <f>200000+30000</f>
+        <v>230000</v>
+      </c>
+      <c r="I14" t="s">
+        <v>1</v>
+      </c>
+      <c r="J14" t="s">
+        <v>2</v>
+      </c>
+      <c r="K14">
+        <f>($H14/$B$12+1)*$B$3</f>
+        <v>5.7272727272727275</v>
+      </c>
+      <c r="L14" t="s">
+        <v>0</v>
+      </c>
+      <c r="M14" t="s">
+        <v>9</v>
+      </c>
+      <c r="N14" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>